<commit_message>
Amélioration du design et du error handling
Fixed a bug where the sender name was my name
</commit_message>
<xml_diff>
--- a/testedugradepython.xlsx
+++ b/testedugradepython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrerey/PycharmProjects/Edugradeexceltopdftomail/graphtutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D10292-9463-564E-9BFF-E49235F1FC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F501B3-EFFE-BB49-B8ED-14B804F791C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{601EFD08-FEDD-455B-BFF1-D4C64D3A2D39}"/>
   </bookViews>
@@ -71,16 +71,16 @@
     <t>XXX , Somewhere  in the world</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Forename</t>
-  </si>
-  <si>
     <t>Subject1</t>
   </si>
   <si>
     <t>Subject2</t>
+  </si>
+  <si>
+    <t>REY</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
   </si>
 </sst>
 </file>
@@ -286,26 +286,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -354,6 +334,26 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -627,13 +627,13 @@
     <tableColumn id="12" xr3:uid="{79D676EE-B364-8B4C-AB4E-FEF33AE4B048}" name="Subject2" dataDxfId="5"/>
     <tableColumn id="11" xr3:uid="{1F523D53-E5AB-7746-989F-B262AD592958}" name="Crédits ECTS Attendus" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{610F97BF-E837-0D41-9146-70FCEA62F278}" name="Crédits ECTS Total" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{434A6FA4-D9DF-4A4F-B13C-BA728DAC856C}" name="Moyenne Générale" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{434A6FA4-D9DF-4A4F-B13C-BA728DAC856C}" name="Moyenne Générale" dataDxfId="2">
       <calculatedColumnFormula>AVERAGE(Tableau1[[#This Row],[Subject1]:[Subject2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{A09FAD63-E76B-0341-98A0-F65E87718211}" name="Décision du Jury" dataDxfId="2">
+    <tableColumn id="13" xr3:uid="{A09FAD63-E76B-0341-98A0-F65E87718211}" name="Décision du Jury" dataDxfId="1">
       <calculatedColumnFormula>"Vous avez obtenu " &amp; H2 &amp; " crédits ECTS. Vous validez le 1er semestre"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A0D700D3-0E3D-4F4E-BE36-238E101AD962}" name="Commentaire" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{A0D700D3-0E3D-4F4E-BE36-238E101AD962}" name="Commentaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -941,8 +941,8 @@
   </sheetPr>
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -978,10 +978,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>6</v>
@@ -1007,10 +1007,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" s="10">
         <v>12</v>
@@ -1200,18 +1200,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1233,14 +1233,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74EC231A-CC1C-4C51-A96A-6016F4E9A048}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E93F18D6-0A25-4E7D-B0BD-9947AE2852B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1254,4 +1246,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74EC231A-CC1C-4C51-A96A-6016F4E9A048}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>